<commit_message>
A modified file is added
</commit_message>
<xml_diff>
--- a/Pairwise.xlsx
+++ b/Pairwise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c24b61eabbdac2de/Документы/обучение skillfactory/publish/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_38063D7A31C81DA46258DAB5F1D247297D581A2B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCB5514A-DC3E-40D0-B3D6-2B9F7C1E6B86}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_38063D7A31C81DA46258DAB5F1D247297D581A2B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC905347-C63C-400A-A56C-B95E931ABB15}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="708" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,7 +437,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D107" sqref="D107"/>
+      <selection pane="bottomRight" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1929,18 +1929,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
-        <v>106</v>
-      </c>
-      <c r="B107">
-        <v>1</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
-      <c r="D107" s="2">
-        <v>1</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="D107" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>